<commit_message>
Fix "And" where should be "and"
</commit_message>
<xml_diff>
--- a/data/grant.xlsx
+++ b/data/grant.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Country Technical Consultant</t>
   </si>
   <si>
-    <t xml:space="preserve">Cambodia</t>
+    <t xml:space="preserve">KHM</t>
   </si>
   <si>
     <t xml:space="preserve">Provided technical expertise and advice to country partners for building an agrometeorology bulletin in three provinces.</t>
@@ -327,7 +327,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>